<commit_message>
[fix]: fix core algorithm
</commit_message>
<xml_diff>
--- a/CoreCapitalEvaluation.xlsx
+++ b/CoreCapitalEvaluation.xlsx
@@ -14,33 +14,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="65">
-  <si>
-    <t>Eddie</t>
-  </si>
-  <si>
-    <t>Gomez</t>
-  </si>
-  <si>
-    <t>Perez</t>
-  </si>
-  <si>
-    <t>McMilan</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="59">
+  <si>
+    <t>UsuarioPrueba</t>
+  </si>
+  <si>
+    <t>prueba2</t>
+  </si>
+  <si>
+    <t>Prueba3</t>
+  </si>
+  <si>
+    <t>apellido</t>
+  </si>
+  <si>
+    <t>apellido2</t>
+  </si>
+  <si>
+    <t>app</t>
+  </si>
+  <si>
+    <t>DNI</t>
   </si>
   <si>
     <t>Pasaporte</t>
   </si>
   <si>
-    <t>DNI</t>
-  </si>
-  <si>
-    <t>76217659</t>
-  </si>
-  <si>
-    <t>456123</t>
-  </si>
-  <si>
-    <t>165432</t>
+    <t>12234567</t>
+  </si>
+  <si>
+    <t>4564456789</t>
+  </si>
+  <si>
+    <t>1223456754</t>
   </si>
   <si>
     <t>D1. Por favor indica tu género</t>
@@ -100,22 +106,46 @@
     <t>1. Si.</t>
   </si>
   <si>
-    <t>5. Alto.</t>
-  </si>
-  <si>
-    <t>4. Adrenalina.</t>
-  </si>
-  <si>
-    <t>4. Sí, con cierta frecuencia.</t>
+    <t>1. Extremadamente bajo.</t>
+  </si>
+  <si>
+    <t>2. Incertidumbre.</t>
+  </si>
+  <si>
+    <t>1. No, nunca.</t>
   </si>
   <si>
     <t>3. No estoy seguro.</t>
   </si>
   <si>
-    <t>4. Principalmente comisión.</t>
-  </si>
-  <si>
-    <t>5. Muy alto.</t>
+    <t>2. Principalmente salario.</t>
+  </si>
+  <si>
+    <t>1. Muy pequeño.</t>
+  </si>
+  <si>
+    <t>1. Cualquier caída en el valor me haría sentir incómodo(a).</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2. Posibilidad de pérdida muy baja.</t>
+  </si>
+  <si>
+    <t>1. Siempre hacia un riesgo menor.</t>
+  </si>
+  <si>
+    <t>3. Bajo.</t>
+  </si>
+  <si>
+    <t>2. Sí, aunque muy raramente.</t>
+  </si>
+  <si>
+    <t>2. Probablemente más seguridad laboral con un pequeño aumento salarial.</t>
+  </si>
+  <si>
+    <t>3. Combinación equitativa de salario y comisión.</t>
   </si>
   <si>
     <t>2. Pequeño.</t>
@@ -124,64 +154,16 @@
     <t>2. Máximo 5%</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>3. Posibilidad de pérdida moderadamente baja.</t>
-  </si>
-  <si>
-    <t>5. Siempre hacia mayor riesgo.</t>
-  </si>
-  <si>
-    <t>3. Sí, aunque con poca frecuencia.</t>
-  </si>
-  <si>
-    <t>4. Probablemente menos seguridad laboral con un gran aumento salarial.</t>
-  </si>
-  <si>
-    <t>3. Combinación equitativa de salario y comisión.</t>
-  </si>
-  <si>
-    <t>6. Máximo 25%</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3. Sin cambios o cambios sin una dirección clara.</t>
-  </si>
-  <si>
-    <t>1. Extremadamente bajo.</t>
-  </si>
-  <si>
-    <t>1. Peligro.</t>
-  </si>
-  <si>
-    <t>1. No, nunca.</t>
-  </si>
-  <si>
-    <t>1. Definitivamente más seguridad laboral con un pequeño aumento salarial.</t>
-  </si>
-  <si>
-    <t>1. Todo salario.</t>
-  </si>
-  <si>
-    <t>1. Muy pequeño.</t>
-  </si>
-  <si>
-    <t>1. Cualquier caída en el valor me haría sentir incómodo(a).</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>1. Cero, es decir, sin posibilidad de pérdida.</t>
-  </si>
-  <si>
-    <t>1. Siempre hacia un riesgo menor.</t>
+    <t>2. Principalmente hacia un riesgo menor.</t>
   </si>
   <si>
     <t>Agresivo</t>
+  </si>
+  <si>
+    <t>Mod. Agresivo</t>
+  </si>
+  <si>
+    <t>Adverso</t>
   </si>
   <si>
     <t xml:space="preserve">Creado: </t>
@@ -573,1336 +555,1336 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
         <v>56</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" t="s">
+      <c r="I1" t="s">
         <v>58</v>
-      </c>
-      <c r="D1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1">
-        <v>44497.52005787037</v>
+        <v>44497.96084490741</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1">
-        <v>44497.52005787037</v>
+        <v>44497.96084490741</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1">
-        <v>44497.52005787037</v>
+        <v>44497.96084490741</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1">
-        <v>44497.52005787037</v>
+        <v>44497.96084490741</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1">
-        <v>44497.52005787037</v>
+        <v>44497.96084490741</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1">
-        <v>44497.52005787037</v>
+        <v>44497.96084490741</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="1">
-        <v>44497.52005787037</v>
+        <v>44497.96084490741</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="1">
-        <v>44497.52005787037</v>
+        <v>44497.96084490741</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H9">
         <v>3</v>
       </c>
       <c r="I9" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="1">
-        <v>44497.52005787037</v>
+        <v>44497.96084490741</v>
       </c>
       <c r="B10" t="s">
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I10" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="1">
-        <v>44497.52005787037</v>
+        <v>44497.96084490741</v>
       </c>
       <c r="B11" t="s">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H11">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="1">
-        <v>44497.52005787037</v>
+        <v>44497.96084490741</v>
       </c>
       <c r="B12" t="s">
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="1">
-        <v>44497.52005787037</v>
+        <v>44497.96084490741</v>
       </c>
       <c r="B13" t="s">
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1">
-        <v>44497.52005787037</v>
+        <v>44497.96084490741</v>
       </c>
       <c r="B14" t="s">
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H14">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="1">
-        <v>44497.52005787037</v>
+        <v>44497.96084490741</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I15" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="1">
-        <v>44497.52005787037</v>
+        <v>44497.96084490741</v>
       </c>
       <c r="B16" t="s">
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E16" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F16" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H16">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="1">
-        <v>44497.52674768519</v>
+        <v>44497.97325231481</v>
       </c>
       <c r="B17" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G17" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1">
-        <v>44497.52674768519</v>
+        <v>44497.97325231481</v>
       </c>
       <c r="B18" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1">
-        <v>44497.52674768519</v>
+        <v>44497.97325231481</v>
       </c>
       <c r="B19" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F19" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="1">
-        <v>44497.52674768519</v>
+        <v>44497.97325231481</v>
       </c>
       <c r="B20" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G20" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="1">
-        <v>44497.52674768519</v>
+        <v>44497.97325231481</v>
       </c>
       <c r="B21" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G21" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="H21">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I21" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="1">
-        <v>44497.52674768519</v>
+        <v>44497.97325231481</v>
       </c>
       <c r="B22" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F22" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G22" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I22" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="1">
-        <v>44497.52674768519</v>
+        <v>44497.97325231481</v>
       </c>
       <c r="B23" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F23" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G23" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I23" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="1">
-        <v>44497.52674768519</v>
+        <v>44497.97325231481</v>
       </c>
       <c r="B24" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F24" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G24" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I24" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="1">
-        <v>44497.52674768519</v>
+        <v>44497.97325231481</v>
       </c>
       <c r="B25" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G25" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H25">
         <v>3</v>
       </c>
       <c r="I25" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="1">
-        <v>44497.52674768519</v>
+        <v>44497.97325231481</v>
       </c>
       <c r="B26" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F26" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G26" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="H26">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I26" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="1">
-        <v>44497.52674768519</v>
+        <v>44497.97325231481</v>
       </c>
       <c r="B27" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F27" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G27" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="H27">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I27" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="1">
-        <v>44497.52674768519</v>
+        <v>44497.97325231481</v>
       </c>
       <c r="B28" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F28" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G28" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H28">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I28" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="1">
-        <v>44497.52674768519</v>
+        <v>44497.97325231481</v>
       </c>
       <c r="B29" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F29" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G29" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="H29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I29" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="1">
-        <v>44497.52674768519</v>
+        <v>44497.97325231481</v>
       </c>
       <c r="B30" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E30" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F30" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I30" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="1">
-        <v>44497.52674768519</v>
+        <v>44497.97325231481</v>
       </c>
       <c r="B31" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F31" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G31" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I31" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="1">
-        <v>44497.54042824074</v>
+        <v>44497.97670138889</v>
       </c>
       <c r="B32" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D32" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E32" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F32" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G32" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H32">
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="1">
-        <v>44497.54042824074</v>
+        <v>44497.97670138889</v>
       </c>
       <c r="B33" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D33" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E33" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F33" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G33" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H33">
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="1">
-        <v>44497.54042824074</v>
+        <v>44497.97670138889</v>
       </c>
       <c r="B34" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D34" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E34" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F34" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G34" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H34">
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="1">
-        <v>44497.54042824074</v>
+        <v>44497.97670138889</v>
       </c>
       <c r="B35" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E35" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F35" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G35" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H35">
         <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="1">
-        <v>44497.54042824074</v>
+        <v>44497.97670138889</v>
       </c>
       <c r="B36" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E36" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F36" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G36" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H36">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I36" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="1">
-        <v>44497.54042824074</v>
+        <v>44497.97670138889</v>
       </c>
       <c r="B37" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E37" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F37" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G37" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="H37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I37" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="1">
-        <v>44497.54042824074</v>
+        <v>44497.97670138889</v>
       </c>
       <c r="B38" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C38" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E38" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F38" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G38" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I38" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="1">
-        <v>44497.54042824074</v>
+        <v>44497.97670138889</v>
       </c>
       <c r="B39" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D39" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E39" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F39" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G39" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I39" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="1">
-        <v>44497.54042824074</v>
+        <v>44497.97670138889</v>
       </c>
       <c r="B40" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D40" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E40" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F40" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G40" t="s">
+        <v>43</v>
+      </c>
+      <c r="H40">
+        <v>3</v>
+      </c>
+      <c r="I40" t="s">
         <v>49</v>
-      </c>
-      <c r="H40">
-        <v>1</v>
-      </c>
-      <c r="I40" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="1">
-        <v>44497.54042824074</v>
+        <v>44497.97670138889</v>
       </c>
       <c r="B41" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E41" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F41" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G41" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I41" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="1">
-        <v>44497.54042824074</v>
+        <v>44497.97670138889</v>
       </c>
       <c r="B42" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E42" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F42" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G42" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I42" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="1">
-        <v>44497.54042824074</v>
+        <v>44497.97670138889</v>
       </c>
       <c r="B43" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D43" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E43" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F43" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G43" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="H43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I43" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="1">
-        <v>44497.54042824074</v>
+        <v>44497.97670138889</v>
       </c>
       <c r="B44" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D44" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E44" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F44" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G44" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="H44">
         <v>1</v>
       </c>
       <c r="I44" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="1">
-        <v>44497.54042824074</v>
+        <v>44497.97670138889</v>
       </c>
       <c r="B45" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D45" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E45" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F45" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G45" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="H45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I45" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="1">
-        <v>44497.54042824074</v>
+        <v>44497.97670138889</v>
       </c>
       <c r="B46" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E46" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F46" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G46" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="H46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I46" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>